<commit_message>
cleaned defensive actions data
</commit_message>
<xml_diff>
--- a/Datasources/Austin_Away/austin_away_defensive_actions.xlsx
+++ b/Datasources/Austin_Away/austin_away_defensive_actions.xlsx
@@ -1,60 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossh\Projects\CITY_Soccer_Analysis\Datasources\Austin_Away\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00A2C00-1F5F-4C53-8C36-A2B40A057995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Austin Away Defensive Actions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="84">
-  <si>
-    <t>Unnamed: 0_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 1_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 2_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 3_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 4_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 5_level_0</t>
-  </si>
-  <si>
-    <t>Tackles</t>
-  </si>
-  <si>
-    <t>Challenges</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="75">
   <si>
     <t>Blocks</t>
   </si>
   <si>
-    <t>Unnamed: 18_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 19_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 20_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 21_level_0</t>
-  </si>
-  <si>
     <t>Player</t>
   </si>
   <si>
@@ -266,13 +236,22 @@
   </si>
   <si>
     <t>32-103</t>
+  </si>
+  <si>
+    <t>Player ID</t>
+  </si>
+  <si>
+    <t>90s</t>
+  </si>
+  <si>
+    <t>Cha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,13 +314,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -379,7 +366,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -413,6 +400,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -447,9 +435,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -622,151 +611,174 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:23">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="M1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="Q1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="T1" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23">
-      <c r="A4" s="1">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
       </c>
       <c r="C4">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="G4">
         <v>87</v>
@@ -792,6 +804,9 @@
       <c r="N4">
         <v>0</v>
       </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
       <c r="P4">
         <v>0</v>
       </c>
@@ -817,24 +832,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C5">
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="G5">
         <v>3</v>
@@ -860,6 +875,9 @@
       <c r="N5">
         <v>0</v>
       </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
       <c r="P5">
         <v>0</v>
       </c>
@@ -885,24 +903,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="G6">
         <v>80</v>
@@ -956,24 +974,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="G7">
         <v>10</v>
@@ -999,6 +1017,9 @@
       <c r="N7">
         <v>0</v>
       </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
       <c r="P7">
         <v>0</v>
       </c>
@@ -1024,24 +1045,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C8">
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="G8">
         <v>58</v>
@@ -1095,24 +1116,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C9">
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
         <v>61</v>
-      </c>
-      <c r="F9" t="s">
-        <v>73</v>
       </c>
       <c r="G9">
         <v>32</v>
@@ -1138,6 +1159,9 @@
       <c r="N9">
         <v>0</v>
       </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
       <c r="P9">
         <v>0</v>
       </c>
@@ -1163,24 +1187,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C10">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" t="s">
         <v>62</v>
-      </c>
-      <c r="F10" t="s">
-        <v>74</v>
       </c>
       <c r="G10">
         <v>59</v>
@@ -1234,24 +1258,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F11" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="G11">
         <v>31</v>
@@ -1305,24 +1329,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="G12">
         <v>90</v>
@@ -1376,24 +1400,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C13">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="G13">
         <v>16</v>
@@ -1447,24 +1471,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C14">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="G14">
         <v>74</v>
@@ -1490,6 +1514,9 @@
       <c r="N14">
         <v>0</v>
       </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
       <c r="P14">
         <v>0</v>
       </c>
@@ -1515,24 +1542,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" t="s">
         <v>52</v>
       </c>
-      <c r="E15" t="s">
-        <v>64</v>
-      </c>
       <c r="F15" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="G15">
         <v>90</v>
@@ -1586,24 +1613,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C16">
         <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="G16">
         <v>90</v>
@@ -1657,24 +1684,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C17">
         <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="F17" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="G17">
         <v>90</v>
@@ -1700,6 +1727,9 @@
       <c r="N17">
         <v>0</v>
       </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
       <c r="P17">
         <v>0</v>
       </c>
@@ -1725,24 +1755,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="F18" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="G18">
         <v>90</v>
@@ -1769,7 +1799,7 @@
         <v>6</v>
       </c>
       <c r="O18">
-        <v>33.3</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="P18">
         <v>4</v>
@@ -1796,24 +1826,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="F19" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="G19">
         <v>90</v>
@@ -1839,6 +1869,9 @@
       <c r="N19">
         <v>0</v>
       </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
       <c r="P19">
         <v>0</v>
       </c>
@@ -1864,12 +1897,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G20">
         <v>990</v>
@@ -1924,11 +1957,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
multiple cleaning changes, added sql schema
</commit_message>
<xml_diff>
--- a/Datasources/Austin_Away/austin_away_defensive_actions.xlsx
+++ b/Datasources/Austin_Away/austin_away_defensive_actions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossh\Projects\CITY_Soccer_Analysis\Datasources\Austin_Away\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00A2C00-1F5F-4C53-8C36-A2B40A057995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A89DFB-9E49-44B1-B4AE-F2DCC6ECF7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="76">
   <si>
     <t>Blocks</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>Cha</t>
+  </si>
+  <si>
+    <t>Match ID</t>
   </si>
 </sst>
 </file>
@@ -303,11 +306,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,180 +616,183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W20"/>
+  <dimension ref="A1:X20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+      <selection sqref="A1:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="R1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
+    <row r="2" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="R2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="3" spans="1:24" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>38</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>47</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>56</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>87</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
       <c r="I4">
         <v>0</v>
       </c>
@@ -826,37 +833,40 @@
         <v>0</v>
       </c>
       <c r="V4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>39</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>47</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>57</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>3</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
       <c r="I5">
         <v>0</v>
       </c>
@@ -902,103 +912,109 @@
       <c r="W5">
         <v>0</v>
       </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>40</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>48</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>58</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>80</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>4</v>
       </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
       <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
         <v>4</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
         <v>4</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>10</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>40</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>6</v>
       </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
       <c r="R6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U6">
+        <v>2</v>
+      </c>
+      <c r="V6">
         <v>6</v>
       </c>
-      <c r="V6">
-        <v>1</v>
-      </c>
       <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>12</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>38</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>48</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>59</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>10</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
       <c r="I7">
         <v>0</v>
       </c>
@@ -1024,123 +1040,129 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7">
         <v>0</v>
       </c>
       <c r="V7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>41</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>49</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>60</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>58</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O8">
+        <v>2</v>
+      </c>
+      <c r="P8">
         <v>50</v>
       </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
       <c r="Q8">
         <v>1</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V8">
         <v>1</v>
       </c>
       <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>11</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>40</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>49</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>61</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>32</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
       <c r="I9">
         <v>0</v>
       </c>
@@ -1175,7 +1197,7 @@
         <v>0</v>
       </c>
       <c r="T9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U9">
         <v>1</v>
@@ -1184,60 +1206,63 @@
         <v>1</v>
       </c>
       <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>7</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>42</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>50</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>62</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>59</v>
       </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R10">
         <v>0</v>
@@ -1249,64 +1274,67 @@
         <v>0</v>
       </c>
       <c r="U10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W10">
         <v>0</v>
       </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>28</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>40</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>50</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>63</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>31</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>3</v>
       </c>
-      <c r="I11">
-        <v>2</v>
-      </c>
       <c r="J11">
         <v>2</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N11">
+        <v>2</v>
+      </c>
+      <c r="O11">
         <v>3</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>66.7</v>
       </c>
-      <c r="P11">
-        <v>1</v>
-      </c>
       <c r="Q11">
         <v>1</v>
       </c>
@@ -1314,141 +1342,147 @@
         <v>1</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11">
         <v>0</v>
       </c>
       <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
         <v>3</v>
       </c>
-      <c r="V11">
-        <v>0</v>
-      </c>
       <c r="W11">
         <v>0</v>
       </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
         <v>8</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>29</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>10</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>43</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>51</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>64</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>90</v>
-      </c>
-      <c r="H12">
-        <v>3</v>
       </c>
       <c r="I12">
         <v>3</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
         <v>3</v>
       </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
       <c r="M12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
         <v>4</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>25</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>3</v>
       </c>
-      <c r="Q12">
-        <v>1</v>
-      </c>
       <c r="R12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T12">
         <v>1</v>
       </c>
       <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12">
         <v>4</v>
       </c>
-      <c r="V12">
-        <v>1</v>
-      </c>
       <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="X12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
         <v>9</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>30</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>19</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>40</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>51</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>65</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>16</v>
       </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13">
         <v>1</v>
       </c>
       <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
         <v>100</v>
       </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
       <c r="Q13">
         <v>0</v>
       </c>
@@ -1462,51 +1496,54 @@
         <v>0</v>
       </c>
       <c r="U13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W13">
         <v>0</v>
       </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
         <v>10</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>31</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>6</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>44</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>51</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>66</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>74</v>
       </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -1521,79 +1558,82 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S14">
         <v>1</v>
       </c>
       <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
         <v>4</v>
       </c>
-      <c r="U14">
+      <c r="V14">
         <v>5</v>
       </c>
-      <c r="V14">
-        <v>1</v>
-      </c>
       <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
         <v>11</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>32</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>14</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>40</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>52</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>67</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>90</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>7</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>4</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>5</v>
       </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
       <c r="L15">
         <v>1</v>
       </c>
       <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
         <v>6</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>9</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>66.7</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>3</v>
       </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
       <c r="R15">
         <v>0</v>
       </c>
@@ -1601,114 +1641,120 @@
         <v>0</v>
       </c>
       <c r="T15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15">
         <v>8</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>5</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
         <v>12</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>33</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>22</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>45</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>53</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>68</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>90</v>
       </c>
-      <c r="H16">
-        <v>2</v>
-      </c>
       <c r="I16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N16">
         <v>2</v>
       </c>
       <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="P16">
         <v>100</v>
       </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
       <c r="Q16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S16">
         <v>1</v>
       </c>
       <c r="T16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V16">
+        <v>2</v>
+      </c>
+      <c r="W16">
         <v>3</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1">
         <v>13</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>34</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>26</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>40</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>53</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>69</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>90</v>
       </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
       <c r="I17">
         <v>0</v>
       </c>
@@ -1743,70 +1789,73 @@
         <v>0</v>
       </c>
       <c r="T17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U17">
         <v>1</v>
       </c>
       <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17">
         <v>9</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1">
         <v>14</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>35</v>
       </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
         <v>40</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>54</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>70</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>90</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>3</v>
       </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
       <c r="J18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N18">
+        <v>2</v>
+      </c>
+      <c r="O18">
         <v>6</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>33.299999999999997</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>4</v>
       </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
       <c r="R18">
         <v>0</v>
       </c>
@@ -1814,43 +1863,46 @@
         <v>0</v>
       </c>
       <c r="T18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18">
         <v>4</v>
       </c>
-      <c r="V18">
-        <v>2</v>
-      </c>
       <c r="W18">
+        <v>2</v>
+      </c>
+      <c r="X18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1">
         <v>15</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>36</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
         <v>46</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>55</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>71</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>90</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
       <c r="I19">
         <v>0</v>
       </c>
@@ -1896,63 +1948,69 @@
       <c r="W19">
         <v>0</v>
       </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
+    <row r="20" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
         <v>16</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>37</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>990</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>26</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>17</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>15</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>10</v>
       </c>
-      <c r="L20">
-        <v>1</v>
-      </c>
       <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
         <v>19</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>39</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <v>48.7</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <v>20</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <v>9</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <v>3</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <v>6</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>11</v>
       </c>
-      <c r="U20">
+      <c r="V20">
         <v>37</v>
       </c>
-      <c r="V20">
+      <c r="W20">
         <v>26</v>
       </c>
-      <c r="W20">
+      <c r="X20">
         <v>0</v>
       </c>
     </row>

</xml_diff>